<commit_message>
Removed redundant commands for the paper,
</commit_message>
<xml_diff>
--- a/Model/Utils/bamp_empirical_simulated.xlsx
+++ b/Model/Utils/bamp_empirical_simulated.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="102">
   <si>
     <t>subjectIds</t>
   </si>
@@ -341,7 +341,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -351,14 +351,18 @@
     </border>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,66 +397,66 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="3" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2">
@@ -511,7 +515,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
@@ -570,7 +574,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B4">
@@ -629,7 +633,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B5">
@@ -688,7 +692,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B6">
@@ -747,7 +751,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B7">
@@ -806,7 +810,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B8">
@@ -865,7 +869,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B9">
@@ -924,7 +928,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B10">
@@ -983,7 +987,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B11">
@@ -1042,7 +1046,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B12">
@@ -1101,7 +1105,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B13">
@@ -1160,7 +1164,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B14">
@@ -1219,7 +1223,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B15">
@@ -1278,7 +1282,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B16">
@@ -1337,7 +1341,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B17">
@@ -1396,7 +1400,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B18">
@@ -1455,7 +1459,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B19">
@@ -1514,7 +1518,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B20">
@@ -1573,7 +1577,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B21">
@@ -1632,7 +1636,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B22">
@@ -1691,7 +1695,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B23">
@@ -1750,7 +1754,7 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B24">
@@ -1809,7 +1813,7 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B25">
@@ -1868,7 +1872,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B26">
@@ -1927,7 +1931,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B27">
@@ -1986,7 +1990,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B28">
@@ -2045,7 +2049,7 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B29">
@@ -2104,7 +2108,7 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B30">
@@ -2163,7 +2167,7 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B31">
@@ -2222,7 +2226,7 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B32">
@@ -2281,7 +2285,7 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="1" t="s">
+      <c r="A33" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B33">
@@ -2340,7 +2344,7 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B34">
@@ -2399,7 +2403,7 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="1" t="s">
+      <c r="A35" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B35">
@@ -2458,7 +2462,7 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="1" t="s">
+      <c r="A36" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B36">
@@ -2517,7 +2521,7 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="1" t="s">
+      <c r="A37" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B37">
@@ -2576,7 +2580,7 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="1" t="s">
+      <c r="A38" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B38">
@@ -2635,7 +2639,7 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="1" t="s">
+      <c r="A39" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B39">
@@ -2694,7 +2698,7 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="1" t="s">
+      <c r="A40" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B40">
@@ -2753,7 +2757,7 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="1" t="s">
+      <c r="A41" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B41">
@@ -2812,7 +2816,7 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="1" t="s">
+      <c r="A42" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B42">
@@ -2871,7 +2875,7 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="1" t="s">
+      <c r="A43" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B43">
@@ -2930,7 +2934,7 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="1" t="s">
+      <c r="A44" s="3" t="s">
         <v>43</v>
       </c>
       <c r="B44">
@@ -2989,7 +2993,7 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="1" t="s">
+      <c r="A45" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B45">
@@ -3048,7 +3052,7 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="1" t="s">
+      <c r="A46" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B46">
@@ -3107,7 +3111,7 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="1" t="s">
+      <c r="A47" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B47">
@@ -3166,7 +3170,7 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="1" t="s">
+      <c r="A48" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B48">
@@ -3225,7 +3229,7 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="1" t="s">
+      <c r="A49" s="3" t="s">
         <v>48</v>
       </c>
       <c r="B49">
@@ -3284,7 +3288,7 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="1" t="s">
+      <c r="A50" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B50">
@@ -3343,7 +3347,7 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="1" t="s">
+      <c r="A51" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B51">
@@ -3402,7 +3406,7 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="1" t="s">
+      <c r="A52" s="3" t="s">
         <v>51</v>
       </c>
       <c r="B52">
@@ -3461,7 +3465,7 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="1" t="s">
+      <c r="A53" s="3" t="s">
         <v>52</v>
       </c>
       <c r="B53">
@@ -3520,7 +3524,7 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="1" t="s">
+      <c r="A54" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B54">
@@ -3579,7 +3583,7 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="1" t="s">
+      <c r="A55" s="3" t="s">
         <v>54</v>
       </c>
       <c r="B55">
@@ -3638,7 +3642,7 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="1" t="s">
+      <c r="A56" s="3" t="s">
         <v>55</v>
       </c>
       <c r="B56">
@@ -3697,7 +3701,7 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="1" t="s">
+      <c r="A57" s="3" t="s">
         <v>56</v>
       </c>
       <c r="B57">
@@ -3756,7 +3760,7 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="1" t="s">
+      <c r="A58" s="3" t="s">
         <v>57</v>
       </c>
       <c r="B58">
@@ -3815,7 +3819,7 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="1" t="s">
+      <c r="A59" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B59">
@@ -3874,7 +3878,7 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="1" t="s">
+      <c r="A60" s="3" t="s">
         <v>59</v>
       </c>
       <c r="B60">
@@ -3933,7 +3937,7 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="1" t="s">
+      <c r="A61" s="3" t="s">
         <v>60</v>
       </c>
       <c r="B61">
@@ -3992,7 +3996,7 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="1" t="s">
+      <c r="A62" s="3" t="s">
         <v>61</v>
       </c>
       <c r="B62">
@@ -4051,7 +4055,7 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="1" t="s">
+      <c r="A63" s="3" t="s">
         <v>62</v>
       </c>
       <c r="B63">
@@ -4110,7 +4114,7 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="1" t="s">
+      <c r="A64" s="3" t="s">
         <v>63</v>
       </c>
       <c r="B64">
@@ -4169,7 +4173,7 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="1" t="s">
+      <c r="A65" s="3" t="s">
         <v>64</v>
       </c>
       <c r="B65">
@@ -4228,7 +4232,7 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="1" t="s">
+      <c r="A66" s="3" t="s">
         <v>65</v>
       </c>
       <c r="B66">
@@ -4287,7 +4291,7 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="1" t="s">
+      <c r="A67" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B67">
@@ -4346,7 +4350,7 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="1" t="s">
+      <c r="A68" s="3" t="s">
         <v>67</v>
       </c>
       <c r="B68">
@@ -4405,7 +4409,7 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="1" t="s">
+      <c r="A69" s="3" t="s">
         <v>68</v>
       </c>
       <c r="B69">
@@ -4464,7 +4468,7 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="1" t="s">
+      <c r="A70" s="3" t="s">
         <v>69</v>
       </c>
       <c r="B70">
@@ -4523,7 +4527,7 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="1" t="s">
+      <c r="A71" s="3" t="s">
         <v>70</v>
       </c>
       <c r="B71">
@@ -4582,7 +4586,7 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="1" t="s">
+      <c r="A72" s="3" t="s">
         <v>71</v>
       </c>
       <c r="B72">
@@ -4641,7 +4645,7 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="1" t="s">
+      <c r="A73" s="3" t="s">
         <v>72</v>
       </c>
       <c r="B73">
@@ -4700,7 +4704,7 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="1" t="s">
+      <c r="A74" s="3" t="s">
         <v>73</v>
       </c>
       <c r="B74">
@@ -4759,7 +4763,7 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="1" t="s">
+      <c r="A75" s="3" t="s">
         <v>74</v>
       </c>
       <c r="B75">
@@ -4818,7 +4822,7 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="1" t="s">
+      <c r="A76" s="3" t="s">
         <v>75</v>
       </c>
       <c r="B76">
@@ -4877,7 +4881,7 @@
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="1" t="s">
+      <c r="A77" s="3" t="s">
         <v>76</v>
       </c>
       <c r="B77">
@@ -4936,7 +4940,7 @@
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="1" t="s">
+      <c r="A78" s="3" t="s">
         <v>77</v>
       </c>
       <c r="B78">
@@ -4995,7 +4999,7 @@
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="1" t="s">
+      <c r="A79" s="3" t="s">
         <v>78</v>
       </c>
       <c r="B79">
@@ -5054,7 +5058,7 @@
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="1" t="s">
+      <c r="A80" s="3" t="s">
         <v>79</v>
       </c>
       <c r="B80">
@@ -5113,7 +5117,7 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="1" t="s">
+      <c r="A81" s="3" t="s">
         <v>80</v>
       </c>
       <c r="B81">
@@ -5172,7 +5176,7 @@
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="1" t="s">
+      <c r="A82" s="3" t="s">
         <v>81</v>
       </c>
       <c r="B82">
@@ -5231,7 +5235,7 @@
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="1" t="s">
+      <c r="A83" s="3" t="s">
         <v>82</v>
       </c>
       <c r="B83">
@@ -5290,7 +5294,7 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="1" t="s">
+      <c r="A84" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B84">

</xml_diff>